<commit_message>
test data is added fro createProject test
</commit_message>
<xml_diff>
--- a/SeleniumActtimeFrameWork/data/testData.xlsx
+++ b/SeleniumActtimeFrameWork/data/testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="14250" windowHeight="6375"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="294">
   <si>
     <t>Test_ID</t>
   </si>
@@ -208,6 +208,696 @@
   </si>
   <si>
     <t>Aitel_00019er865r</t>
+  </si>
+  <si>
+    <t>tc_23</t>
+  </si>
+  <si>
+    <t>data_23</t>
+  </si>
+  <si>
+    <t>tc_24</t>
+  </si>
+  <si>
+    <t>data_24</t>
+  </si>
+  <si>
+    <t>tc_25</t>
+  </si>
+  <si>
+    <t>data_25</t>
+  </si>
+  <si>
+    <t>tc_26</t>
+  </si>
+  <si>
+    <t>data_26</t>
+  </si>
+  <si>
+    <t>tc_27</t>
+  </si>
+  <si>
+    <t>data_27</t>
+  </si>
+  <si>
+    <t>tc_28</t>
+  </si>
+  <si>
+    <t>data_28</t>
+  </si>
+  <si>
+    <t>tc_29</t>
+  </si>
+  <si>
+    <t>data_29</t>
+  </si>
+  <si>
+    <t>tc_30</t>
+  </si>
+  <si>
+    <t>data_30</t>
+  </si>
+  <si>
+    <t>tc_31</t>
+  </si>
+  <si>
+    <t>data_31</t>
+  </si>
+  <si>
+    <t>tc_32</t>
+  </si>
+  <si>
+    <t>data_32</t>
+  </si>
+  <si>
+    <t>tc_33</t>
+  </si>
+  <si>
+    <t>data_33</t>
+  </si>
+  <si>
+    <t>tc_34</t>
+  </si>
+  <si>
+    <t>data_34</t>
+  </si>
+  <si>
+    <t>tc_35</t>
+  </si>
+  <si>
+    <t>data_35</t>
+  </si>
+  <si>
+    <t>tc_36</t>
+  </si>
+  <si>
+    <t>data_36</t>
+  </si>
+  <si>
+    <t>tc_37</t>
+  </si>
+  <si>
+    <t>data_37</t>
+  </si>
+  <si>
+    <t>tc_38</t>
+  </si>
+  <si>
+    <t>data_38</t>
+  </si>
+  <si>
+    <t>tc_39</t>
+  </si>
+  <si>
+    <t>data_39</t>
+  </si>
+  <si>
+    <t>tc_40</t>
+  </si>
+  <si>
+    <t>data_40</t>
+  </si>
+  <si>
+    <t>tc_41</t>
+  </si>
+  <si>
+    <t>data_41</t>
+  </si>
+  <si>
+    <t>tc_42</t>
+  </si>
+  <si>
+    <t>data_42</t>
+  </si>
+  <si>
+    <t>tc_43</t>
+  </si>
+  <si>
+    <t>data_43</t>
+  </si>
+  <si>
+    <t>tc_44</t>
+  </si>
+  <si>
+    <t>data_44</t>
+  </si>
+  <si>
+    <t>tc_45</t>
+  </si>
+  <si>
+    <t>data_45</t>
+  </si>
+  <si>
+    <t>tc_46</t>
+  </si>
+  <si>
+    <t>data_46</t>
+  </si>
+  <si>
+    <t>tc_47</t>
+  </si>
+  <si>
+    <t>data_47</t>
+  </si>
+  <si>
+    <t>tc_48</t>
+  </si>
+  <si>
+    <t>data_48</t>
+  </si>
+  <si>
+    <t>tc_49</t>
+  </si>
+  <si>
+    <t>data_49</t>
+  </si>
+  <si>
+    <t>tc_50</t>
+  </si>
+  <si>
+    <t>data_50</t>
+  </si>
+  <si>
+    <t>tc_51</t>
+  </si>
+  <si>
+    <t>data_51</t>
+  </si>
+  <si>
+    <t>tc_52</t>
+  </si>
+  <si>
+    <t>data_52</t>
+  </si>
+  <si>
+    <t>tc_53</t>
+  </si>
+  <si>
+    <t>data_53</t>
+  </si>
+  <si>
+    <t>tc_54</t>
+  </si>
+  <si>
+    <t>data_54</t>
+  </si>
+  <si>
+    <t>tc_55</t>
+  </si>
+  <si>
+    <t>data_55</t>
+  </si>
+  <si>
+    <t>tc_56</t>
+  </si>
+  <si>
+    <t>data_56</t>
+  </si>
+  <si>
+    <t>tc_57</t>
+  </si>
+  <si>
+    <t>data_57</t>
+  </si>
+  <si>
+    <t>tc_58</t>
+  </si>
+  <si>
+    <t>data_58</t>
+  </si>
+  <si>
+    <t>tc_59</t>
+  </si>
+  <si>
+    <t>data_59</t>
+  </si>
+  <si>
+    <t>tc_60</t>
+  </si>
+  <si>
+    <t>data_60</t>
+  </si>
+  <si>
+    <t>tc_61</t>
+  </si>
+  <si>
+    <t>data_61</t>
+  </si>
+  <si>
+    <t>tc_62</t>
+  </si>
+  <si>
+    <t>data_62</t>
+  </si>
+  <si>
+    <t>tc_63</t>
+  </si>
+  <si>
+    <t>data_63</t>
+  </si>
+  <si>
+    <t>tc_64</t>
+  </si>
+  <si>
+    <t>data_64</t>
+  </si>
+  <si>
+    <t>tc_65</t>
+  </si>
+  <si>
+    <t>data_65</t>
+  </si>
+  <si>
+    <t>tc_66</t>
+  </si>
+  <si>
+    <t>data_66</t>
+  </si>
+  <si>
+    <t>tc_67</t>
+  </si>
+  <si>
+    <t>data_67</t>
+  </si>
+  <si>
+    <t>tc_68</t>
+  </si>
+  <si>
+    <t>data_68</t>
+  </si>
+  <si>
+    <t>tc_69</t>
+  </si>
+  <si>
+    <t>data_69</t>
+  </si>
+  <si>
+    <t>tc_70</t>
+  </si>
+  <si>
+    <t>data_70</t>
+  </si>
+  <si>
+    <t>tc_71</t>
+  </si>
+  <si>
+    <t>data_71</t>
+  </si>
+  <si>
+    <t>tc_72</t>
+  </si>
+  <si>
+    <t>data_72</t>
+  </si>
+  <si>
+    <t>tc_73</t>
+  </si>
+  <si>
+    <t>data_73</t>
+  </si>
+  <si>
+    <t>tc_74</t>
+  </si>
+  <si>
+    <t>data_74</t>
+  </si>
+  <si>
+    <t>tc_75</t>
+  </si>
+  <si>
+    <t>data_75</t>
+  </si>
+  <si>
+    <t>tc_76</t>
+  </si>
+  <si>
+    <t>data_76</t>
+  </si>
+  <si>
+    <t>tc_77</t>
+  </si>
+  <si>
+    <t>data_77</t>
+  </si>
+  <si>
+    <t>tc_78</t>
+  </si>
+  <si>
+    <t>data_78</t>
+  </si>
+  <si>
+    <t>tc_79</t>
+  </si>
+  <si>
+    <t>data_79</t>
+  </si>
+  <si>
+    <t>tc_80</t>
+  </si>
+  <si>
+    <t>data_80</t>
+  </si>
+  <si>
+    <t>tc_81</t>
+  </si>
+  <si>
+    <t>data_81</t>
+  </si>
+  <si>
+    <t>tc_82</t>
+  </si>
+  <si>
+    <t>data_82</t>
+  </si>
+  <si>
+    <t>tc_83</t>
+  </si>
+  <si>
+    <t>data_83</t>
+  </si>
+  <si>
+    <t>tc_84</t>
+  </si>
+  <si>
+    <t>data_84</t>
+  </si>
+  <si>
+    <t>tc_85</t>
+  </si>
+  <si>
+    <t>data_85</t>
+  </si>
+  <si>
+    <t>tc_86</t>
+  </si>
+  <si>
+    <t>data_86</t>
+  </si>
+  <si>
+    <t>tc_87</t>
+  </si>
+  <si>
+    <t>data_87</t>
+  </si>
+  <si>
+    <t>tc_88</t>
+  </si>
+  <si>
+    <t>data_88</t>
+  </si>
+  <si>
+    <t>tc_89</t>
+  </si>
+  <si>
+    <t>data_89</t>
+  </si>
+  <si>
+    <t>tc_90</t>
+  </si>
+  <si>
+    <t>data_90</t>
+  </si>
+  <si>
+    <t>tc_91</t>
+  </si>
+  <si>
+    <t>data_91</t>
+  </si>
+  <si>
+    <t>tc_92</t>
+  </si>
+  <si>
+    <t>data_92</t>
+  </si>
+  <si>
+    <t>tc_93</t>
+  </si>
+  <si>
+    <t>data_93</t>
+  </si>
+  <si>
+    <t>tc_94</t>
+  </si>
+  <si>
+    <t>data_94</t>
+  </si>
+  <si>
+    <t>tc_95</t>
+  </si>
+  <si>
+    <t>data_95</t>
+  </si>
+  <si>
+    <t>tc_96</t>
+  </si>
+  <si>
+    <t>data_96</t>
+  </si>
+  <si>
+    <t>tc_97</t>
+  </si>
+  <si>
+    <t>data_97</t>
+  </si>
+  <si>
+    <t>tc_98</t>
+  </si>
+  <si>
+    <t>data_98</t>
+  </si>
+  <si>
+    <t>tc_99</t>
+  </si>
+  <si>
+    <t>data_99</t>
+  </si>
+  <si>
+    <t>tc_100</t>
+  </si>
+  <si>
+    <t>data_100</t>
+  </si>
+  <si>
+    <t>tc_101</t>
+  </si>
+  <si>
+    <t>data_101</t>
+  </si>
+  <si>
+    <t>tc_102</t>
+  </si>
+  <si>
+    <t>data_102</t>
+  </si>
+  <si>
+    <t>tc_103</t>
+  </si>
+  <si>
+    <t>data_103</t>
+  </si>
+  <si>
+    <t>tc_104</t>
+  </si>
+  <si>
+    <t>data_104</t>
+  </si>
+  <si>
+    <t>tc_105</t>
+  </si>
+  <si>
+    <t>data_105</t>
+  </si>
+  <si>
+    <t>tc_106</t>
+  </si>
+  <si>
+    <t>data_106</t>
+  </si>
+  <si>
+    <t>tc_107</t>
+  </si>
+  <si>
+    <t>data_107</t>
+  </si>
+  <si>
+    <t>tc_108</t>
+  </si>
+  <si>
+    <t>data_108</t>
+  </si>
+  <si>
+    <t>tc_109</t>
+  </si>
+  <si>
+    <t>data_109</t>
+  </si>
+  <si>
+    <t>tc_110</t>
+  </si>
+  <si>
+    <t>data_110</t>
+  </si>
+  <si>
+    <t>tc_111</t>
+  </si>
+  <si>
+    <t>data_111</t>
+  </si>
+  <si>
+    <t>tc_112</t>
+  </si>
+  <si>
+    <t>data_112</t>
+  </si>
+  <si>
+    <t>tc_113</t>
+  </si>
+  <si>
+    <t>data_113</t>
+  </si>
+  <si>
+    <t>tc_114</t>
+  </si>
+  <si>
+    <t>data_114</t>
+  </si>
+  <si>
+    <t>tc_115</t>
+  </si>
+  <si>
+    <t>data_115</t>
+  </si>
+  <si>
+    <t>tc_116</t>
+  </si>
+  <si>
+    <t>data_116</t>
+  </si>
+  <si>
+    <t>tc_117</t>
+  </si>
+  <si>
+    <t>data_117</t>
+  </si>
+  <si>
+    <t>tc_118</t>
+  </si>
+  <si>
+    <t>data_118</t>
+  </si>
+  <si>
+    <t>tc_119</t>
+  </si>
+  <si>
+    <t>data_119</t>
+  </si>
+  <si>
+    <t>tc_120</t>
+  </si>
+  <si>
+    <t>data_120</t>
+  </si>
+  <si>
+    <t>tc_121</t>
+  </si>
+  <si>
+    <t>data_121</t>
+  </si>
+  <si>
+    <t>tc_122</t>
+  </si>
+  <si>
+    <t>data_122</t>
+  </si>
+  <si>
+    <t>tc_123</t>
+  </si>
+  <si>
+    <t>data_123</t>
+  </si>
+  <si>
+    <t>tc_124</t>
+  </si>
+  <si>
+    <t>data_124</t>
+  </si>
+  <si>
+    <t>tc_125</t>
+  </si>
+  <si>
+    <t>data_125</t>
+  </si>
+  <si>
+    <t>tc_126</t>
+  </si>
+  <si>
+    <t>data_126</t>
+  </si>
+  <si>
+    <t>tc_127</t>
+  </si>
+  <si>
+    <t>data_127</t>
+  </si>
+  <si>
+    <t>tc_128</t>
+  </si>
+  <si>
+    <t>data_128</t>
+  </si>
+  <si>
+    <t>tc_129</t>
+  </si>
+  <si>
+    <t>data_129</t>
+  </si>
+  <si>
+    <t>tc_130</t>
+  </si>
+  <si>
+    <t>data_130</t>
+  </si>
+  <si>
+    <t>tc_131</t>
+  </si>
+  <si>
+    <t>data_131</t>
+  </si>
+  <si>
+    <t>tc_132</t>
+  </si>
+  <si>
+    <t>data_132</t>
+  </si>
+  <si>
+    <t>tc_133</t>
+  </si>
+  <si>
+    <t>data_133</t>
+  </si>
+  <si>
+    <t>tc_134</t>
+  </si>
+  <si>
+    <t>data_134</t>
+  </si>
+  <si>
+    <t>tc_135</t>
+  </si>
+  <si>
+    <t>data_135</t>
+  </si>
+  <si>
+    <t>customerName</t>
+  </si>
+  <si>
+    <t>projectName</t>
+  </si>
+  <si>
+    <t>AA_BB_CCC</t>
+  </si>
+  <si>
+    <t>support</t>
   </si>
 </sst>
 </file>
@@ -563,10 +1253,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -680,6 +1370,38 @@
         <v>61</v>
       </c>
     </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -688,10 +1410,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E135"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView topLeftCell="A8" zoomScale="145" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C134" sqref="C134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -873,6 +1595,910 @@
       </c>
       <c r="B22" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>76</v>
+      </c>
+      <c r="B29" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>78</v>
+      </c>
+      <c r="B30" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>82</v>
+      </c>
+      <c r="B32" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>84</v>
+      </c>
+      <c r="B33" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>86</v>
+      </c>
+      <c r="B34" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>88</v>
+      </c>
+      <c r="B35" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>90</v>
+      </c>
+      <c r="B36" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>92</v>
+      </c>
+      <c r="B37" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>94</v>
+      </c>
+      <c r="B38" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>96</v>
+      </c>
+      <c r="B39" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>98</v>
+      </c>
+      <c r="B40" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>100</v>
+      </c>
+      <c r="B41" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>102</v>
+      </c>
+      <c r="B42" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>104</v>
+      </c>
+      <c r="B43" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>106</v>
+      </c>
+      <c r="B44" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>108</v>
+      </c>
+      <c r="B45" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>110</v>
+      </c>
+      <c r="B46" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>112</v>
+      </c>
+      <c r="B47" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>114</v>
+      </c>
+      <c r="B48" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>116</v>
+      </c>
+      <c r="B49" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>118</v>
+      </c>
+      <c r="B50" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>120</v>
+      </c>
+      <c r="B51" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>122</v>
+      </c>
+      <c r="B52" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>124</v>
+      </c>
+      <c r="B53" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>126</v>
+      </c>
+      <c r="B54" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>128</v>
+      </c>
+      <c r="B55" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>130</v>
+      </c>
+      <c r="B56" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>132</v>
+      </c>
+      <c r="B57" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>134</v>
+      </c>
+      <c r="B58" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>136</v>
+      </c>
+      <c r="B59" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>138</v>
+      </c>
+      <c r="B60" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
+        <v>140</v>
+      </c>
+      <c r="B61" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
+        <v>142</v>
+      </c>
+      <c r="B62" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
+        <v>144</v>
+      </c>
+      <c r="B63" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
+        <v>146</v>
+      </c>
+      <c r="B64" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>148</v>
+      </c>
+      <c r="B65" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>150</v>
+      </c>
+      <c r="B66" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
+        <v>152</v>
+      </c>
+      <c r="B67" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" t="s">
+        <v>154</v>
+      </c>
+      <c r="B68" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
+        <v>156</v>
+      </c>
+      <c r="B69" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
+        <v>158</v>
+      </c>
+      <c r="B70" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
+        <v>160</v>
+      </c>
+      <c r="B71" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
+        <v>162</v>
+      </c>
+      <c r="B72" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
+        <v>164</v>
+      </c>
+      <c r="B73" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
+        <v>166</v>
+      </c>
+      <c r="B74" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
+        <v>168</v>
+      </c>
+      <c r="B75" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>170</v>
+      </c>
+      <c r="B76" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
+        <v>172</v>
+      </c>
+      <c r="B77" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
+        <v>174</v>
+      </c>
+      <c r="B78" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
+        <v>176</v>
+      </c>
+      <c r="B79" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
+        <v>178</v>
+      </c>
+      <c r="B80" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
+        <v>180</v>
+      </c>
+      <c r="B81" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" t="s">
+        <v>182</v>
+      </c>
+      <c r="B82" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" t="s">
+        <v>184</v>
+      </c>
+      <c r="B83" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" t="s">
+        <v>186</v>
+      </c>
+      <c r="B84" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" t="s">
+        <v>188</v>
+      </c>
+      <c r="B85" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" t="s">
+        <v>190</v>
+      </c>
+      <c r="B86" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" t="s">
+        <v>192</v>
+      </c>
+      <c r="B87" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" t="s">
+        <v>194</v>
+      </c>
+      <c r="B88" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" t="s">
+        <v>196</v>
+      </c>
+      <c r="B89" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" t="s">
+        <v>198</v>
+      </c>
+      <c r="B90" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" t="s">
+        <v>200</v>
+      </c>
+      <c r="B91" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" t="s">
+        <v>202</v>
+      </c>
+      <c r="B92" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" t="s">
+        <v>204</v>
+      </c>
+      <c r="B93" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" t="s">
+        <v>206</v>
+      </c>
+      <c r="B94" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" t="s">
+        <v>208</v>
+      </c>
+      <c r="B95" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" t="s">
+        <v>210</v>
+      </c>
+      <c r="B96" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" t="s">
+        <v>212</v>
+      </c>
+      <c r="B97" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" t="s">
+        <v>214</v>
+      </c>
+      <c r="B98" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" t="s">
+        <v>216</v>
+      </c>
+      <c r="B99" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" t="s">
+        <v>218</v>
+      </c>
+      <c r="B100" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" t="s">
+        <v>220</v>
+      </c>
+      <c r="B101" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" t="s">
+        <v>222</v>
+      </c>
+      <c r="B102" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" t="s">
+        <v>224</v>
+      </c>
+      <c r="B103" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" t="s">
+        <v>226</v>
+      </c>
+      <c r="B104" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" t="s">
+        <v>228</v>
+      </c>
+      <c r="B105" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" t="s">
+        <v>230</v>
+      </c>
+      <c r="B106" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" t="s">
+        <v>232</v>
+      </c>
+      <c r="B107" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" t="s">
+        <v>234</v>
+      </c>
+      <c r="B108" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" t="s">
+        <v>236</v>
+      </c>
+      <c r="B109" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" t="s">
+        <v>238</v>
+      </c>
+      <c r="B110" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" t="s">
+        <v>240</v>
+      </c>
+      <c r="B111" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" t="s">
+        <v>242</v>
+      </c>
+      <c r="B112" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" t="s">
+        <v>244</v>
+      </c>
+      <c r="B113" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" t="s">
+        <v>246</v>
+      </c>
+      <c r="B114" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" t="s">
+        <v>248</v>
+      </c>
+      <c r="B115" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" t="s">
+        <v>250</v>
+      </c>
+      <c r="B116" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" t="s">
+        <v>252</v>
+      </c>
+      <c r="B117" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" t="s">
+        <v>254</v>
+      </c>
+      <c r="B118" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" t="s">
+        <v>256</v>
+      </c>
+      <c r="B119" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" t="s">
+        <v>258</v>
+      </c>
+      <c r="B120" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" t="s">
+        <v>260</v>
+      </c>
+      <c r="B121" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" t="s">
+        <v>262</v>
+      </c>
+      <c r="B122" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" t="s">
+        <v>264</v>
+      </c>
+      <c r="B123" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" t="s">
+        <v>266</v>
+      </c>
+      <c r="B124" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" t="s">
+        <v>268</v>
+      </c>
+      <c r="B125" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" t="s">
+        <v>270</v>
+      </c>
+      <c r="B126" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" t="s">
+        <v>272</v>
+      </c>
+      <c r="B127" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" t="s">
+        <v>274</v>
+      </c>
+      <c r="B128" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129" t="s">
+        <v>276</v>
+      </c>
+      <c r="B129" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130" t="s">
+        <v>278</v>
+      </c>
+      <c r="B130" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" t="s">
+        <v>280</v>
+      </c>
+      <c r="B131" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="A132" t="s">
+        <v>282</v>
+      </c>
+      <c r="B132" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="A133" t="s">
+        <v>284</v>
+      </c>
+      <c r="B133" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="A134" t="s">
+        <v>286</v>
+      </c>
+      <c r="B134" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="A135" t="s">
+        <v>288</v>
+      </c>
+      <c r="B135" t="s">
+        <v>289</v>
       </c>
     </row>
   </sheetData>

</xml_diff>